<commit_message>
Update Sam model design
</commit_message>
<xml_diff>
--- a/ImportONNXNetworkAsFunctionExample/Sam_h.XLSX
+++ b/ImportONNXNetworkAsFunctionExample/Sam_h.XLSX
@@ -8,13 +8,16 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Git\Spectrum_sensing_base_on_Deep_learning\ImportONNXNetworkAsFunctionExample\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{ACCFCD79-BE9A-4166-B747-56055F437A6A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2226BAC6-B7B5-45D7-AFBE-984E7CE31C48}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Connection" sheetId="1" r:id="rId1"/>
-    <sheet name="Layers" sheetId="2" r:id="rId2"/>
+    <sheet name="learnable" sheetId="3" r:id="rId2"/>
+    <sheet name="InputName" sheetId="4" r:id="rId3"/>
+    <sheet name="OutputName" sheetId="5" r:id="rId4"/>
+    <sheet name="Layers" sheetId="2" r:id="rId5"/>
   </sheets>
   <calcPr calcId="162913"/>
   <extLst>
@@ -26,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="154" uniqueCount="105">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="778" uniqueCount="308">
   <si>
     <t>'image_embeddings/image_embeddings'</t>
   </si>
@@ -341,6 +344,615 @@
   </si>
   <si>
     <t>1x1 CustomOutputLayer</t>
+  </si>
+  <si>
+    <t>undefined</t>
+  </si>
+  <si>
+    <t>Unsqueeze_To_ReshapeLayer1127</t>
+  </si>
+  <si>
+    <t>mask_decoder_outp_13</t>
+  </si>
+  <si>
+    <t>256x256 dlarray</t>
+  </si>
+  <si>
+    <t>mask_decoder_outp_14</t>
+  </si>
+  <si>
+    <t>256x1 dlarray</t>
+  </si>
+  <si>
+    <t>mask_decoder_outp_15</t>
+  </si>
+  <si>
+    <t>mask_decoder_outp_16</t>
+  </si>
+  <si>
+    <t>32x1 dlarray</t>
+  </si>
+  <si>
+    <t>mask_decoder_outp_17</t>
+  </si>
+  <si>
+    <t>256x32 dlarray</t>
+  </si>
+  <si>
+    <t>mask_decoder_outp_18</t>
+  </si>
+  <si>
+    <t>mask_decoder_outp_19</t>
+  </si>
+  <si>
+    <t>mask_decoder_outp_2</t>
+  </si>
+  <si>
+    <t>mask_decoder_outp_20</t>
+  </si>
+  <si>
+    <t>mask_decoder_outp_21</t>
+  </si>
+  <si>
+    <t>mask_decoder_outp_22</t>
+  </si>
+  <si>
+    <t>mask_decoder_outp_23</t>
+  </si>
+  <si>
+    <t>mask_decoder_outp_3</t>
+  </si>
+  <si>
+    <t>mask_decoder_outp_4</t>
+  </si>
+  <si>
+    <t>mask_decoder_outp_5</t>
+  </si>
+  <si>
+    <t>mask_decoder_outp_6</t>
+  </si>
+  <si>
+    <t>mask_decoder_outp_7</t>
+  </si>
+  <si>
+    <t>mask_decoder_outp_8</t>
+  </si>
+  <si>
+    <t>mask_decoder_outp_9</t>
+  </si>
+  <si>
+    <t>mask_decoder_output_</t>
+  </si>
+  <si>
+    <t>mask_decoder_tran_14</t>
+  </si>
+  <si>
+    <t>mask_decoder_tran_15</t>
+  </si>
+  <si>
+    <t>mask_decoder_tran_16</t>
+  </si>
+  <si>
+    <t>mask_decoder_tran_17</t>
+  </si>
+  <si>
+    <t>mask_decoder_tran_18</t>
+  </si>
+  <si>
+    <t>mask_decoder_tran_19</t>
+  </si>
+  <si>
+    <t>mask_decoder_tran_20</t>
+  </si>
+  <si>
+    <t>mask_decoder_tran_21</t>
+  </si>
+  <si>
+    <t>mask_decoder_tran_36</t>
+  </si>
+  <si>
+    <t>mask_decoder_tran_37</t>
+  </si>
+  <si>
+    <t>mask_decoder_tran_38</t>
+  </si>
+  <si>
+    <t>mask_decoder_tran_39</t>
+  </si>
+  <si>
+    <t>mask_decoder_tran_40</t>
+  </si>
+  <si>
+    <t>mask_decoder_tran_41</t>
+  </si>
+  <si>
+    <t>mask_decoder_tran_42</t>
+  </si>
+  <si>
+    <t>mask_decoder_tran_43</t>
+  </si>
+  <si>
+    <t>mask_decoder_tran_48</t>
+  </si>
+  <si>
+    <t>mask_decoder_tran_49</t>
+  </si>
+  <si>
+    <t>model_prompt_enco_7</t>
+  </si>
+  <si>
+    <t>128x2 dlarray</t>
+  </si>
+  <si>
+    <t>onnx__Expand_1853</t>
+  </si>
+  <si>
+    <t>256x5 dlarray</t>
+  </si>
+  <si>
+    <t>onnx__MatMul_1858</t>
+  </si>
+  <si>
+    <t>onnx__MatMul_1859</t>
+  </si>
+  <si>
+    <t>onnx__MatMul_1860</t>
+  </si>
+  <si>
+    <t>onnx__MatMul_1864</t>
+  </si>
+  <si>
+    <t>onnx__MatMul_1865</t>
+  </si>
+  <si>
+    <t>128x256 dlarray</t>
+  </si>
+  <si>
+    <t>onnx__MatMul_1866</t>
+  </si>
+  <si>
+    <t>onnx__MatMul_1867</t>
+  </si>
+  <si>
+    <t>onnx__MatMul_1871</t>
+  </si>
+  <si>
+    <t>256x128 dlarray</t>
+  </si>
+  <si>
+    <t>onnx__MatMul_1872</t>
+  </si>
+  <si>
+    <t>2048x256 dlarray</t>
+  </si>
+  <si>
+    <t>onnx__MatMul_1873</t>
+  </si>
+  <si>
+    <t>256x2048 dlarray</t>
+  </si>
+  <si>
+    <t>onnx__MatMul_1874</t>
+  </si>
+  <si>
+    <t>onnx__MatMul_1875</t>
+  </si>
+  <si>
+    <t>onnx__MatMul_1876</t>
+  </si>
+  <si>
+    <t>onnx__MatMul_1880</t>
+  </si>
+  <si>
+    <t>onnx__MatMul_1881</t>
+  </si>
+  <si>
+    <t>onnx__MatMul_1882</t>
+  </si>
+  <si>
+    <t>onnx__MatMul_1883</t>
+  </si>
+  <si>
+    <t>onnx__MatMul_1887</t>
+  </si>
+  <si>
+    <t>onnx__MatMul_1888</t>
+  </si>
+  <si>
+    <t>onnx__MatMul_1889</t>
+  </si>
+  <si>
+    <t>onnx__MatMul_1890</t>
+  </si>
+  <si>
+    <t>onnx__MatMul_1894</t>
+  </si>
+  <si>
+    <t>onnx__MatMul_1895</t>
+  </si>
+  <si>
+    <t>onnx__MatMul_1896</t>
+  </si>
+  <si>
+    <t>onnx__MatMul_1897</t>
+  </si>
+  <si>
+    <t>onnx__MatMul_1898</t>
+  </si>
+  <si>
+    <t>onnx__MatMul_1899</t>
+  </si>
+  <si>
+    <t>onnx__MatMul_1903</t>
+  </si>
+  <si>
+    <t>onnx__MatMul_1904</t>
+  </si>
+  <si>
+    <t>onnx__MatMul_1905</t>
+  </si>
+  <si>
+    <t>onnx__MatMul_1906</t>
+  </si>
+  <si>
+    <t>onnx__MatMul_1910</t>
+  </si>
+  <si>
+    <t>onnx__Unsqueeze_1009</t>
+  </si>
+  <si>
+    <t>1x1     dlarray</t>
+  </si>
+  <si>
+    <t>onnx__Unsqueeze_1011</t>
+  </si>
+  <si>
+    <t>onnx__Unsqueeze_1015</t>
+  </si>
+  <si>
+    <t>onnx__Unsqueeze_1032</t>
+  </si>
+  <si>
+    <t>onnx__Unsqueeze_1034</t>
+  </si>
+  <si>
+    <t>onnx__Unsqueeze_1038</t>
+  </si>
+  <si>
+    <t>onnx__Unsqueeze_1063</t>
+  </si>
+  <si>
+    <t>onnx__Unsqueeze_1065</t>
+  </si>
+  <si>
+    <t>onnx__Unsqueeze_1067</t>
+  </si>
+  <si>
+    <t>onnx__Unsqueeze_1108</t>
+  </si>
+  <si>
+    <t>onnx__Unsqueeze_1110</t>
+  </si>
+  <si>
+    <t>onnx__Unsqueeze_1114</t>
+  </si>
+  <si>
+    <t>onnx__Unsqueeze_1132</t>
+  </si>
+  <si>
+    <t>onnx__Unsqueeze_1134</t>
+  </si>
+  <si>
+    <t>onnx__Unsqueeze_1138</t>
+  </si>
+  <si>
+    <t>onnx__Unsqueeze_1155</t>
+  </si>
+  <si>
+    <t>onnx__Unsqueeze_1157</t>
+  </si>
+  <si>
+    <t>onnx__Unsqueeze_1161</t>
+  </si>
+  <si>
+    <t>onnx__Unsqueeze_1186</t>
+  </si>
+  <si>
+    <t>onnx__Unsqueeze_1188</t>
+  </si>
+  <si>
+    <t>onnx__Unsqueeze_1190</t>
+  </si>
+  <si>
+    <t>onnx__Unsqueeze_1221</t>
+  </si>
+  <si>
+    <t>onnx__Unsqueeze_1223</t>
+  </si>
+  <si>
+    <t>onnx__Unsqueeze_1227</t>
+  </si>
+  <si>
+    <t>onnx__Unsqueeze_1245</t>
+  </si>
+  <si>
+    <t>onnx__Unsqueeze_1247</t>
+  </si>
+  <si>
+    <t>onnx__Unsqueeze_1251</t>
+  </si>
+  <si>
+    <t>onnx__Unsqueeze_1268</t>
+  </si>
+  <si>
+    <t>onnx__Unsqueeze_1270</t>
+  </si>
+  <si>
+    <t>onnx__Unsqueeze_1274</t>
+  </si>
+  <si>
+    <t>onnx__Unsqueeze_1299</t>
+  </si>
+  <si>
+    <t>onnx__Unsqueeze_1301</t>
+  </si>
+  <si>
+    <t>onnx__Unsqueeze_1303</t>
+  </si>
+  <si>
+    <t>onnx__Unsqueeze_1336</t>
+  </si>
+  <si>
+    <t>onnx__Unsqueeze_1338</t>
+  </si>
+  <si>
+    <t>onnx__Unsqueeze_1342</t>
+  </si>
+  <si>
+    <t>onnx__Unsqueeze_1360</t>
+  </si>
+  <si>
+    <t>onnx__Unsqueeze_1362</t>
+  </si>
+  <si>
+    <t>onnx__Unsqueeze_1366</t>
+  </si>
+  <si>
+    <t>onnx__Unsqueeze_1383</t>
+  </si>
+  <si>
+    <t>onnx__Unsqueeze_1385</t>
+  </si>
+  <si>
+    <t>onnx__Unsqueeze_1389</t>
+  </si>
+  <si>
+    <t>onnx__Unsqueeze_1414</t>
+  </si>
+  <si>
+    <t>onnx__Unsqueeze_1416</t>
+  </si>
+  <si>
+    <t>onnx__Unsqueeze_1418</t>
+  </si>
+  <si>
+    <t>onnx__Unsqueeze_1459</t>
+  </si>
+  <si>
+    <t>onnx__Unsqueeze_1461</t>
+  </si>
+  <si>
+    <t>onnx__Unsqueeze_1465</t>
+  </si>
+  <si>
+    <t>onnx__Unsqueeze_1483</t>
+  </si>
+  <si>
+    <t>onnx__Unsqueeze_1485</t>
+  </si>
+  <si>
+    <t>onnx__Unsqueeze_1489</t>
+  </si>
+  <si>
+    <t>onnx__Unsqueeze_1506</t>
+  </si>
+  <si>
+    <t>onnx__Unsqueeze_1508</t>
+  </si>
+  <si>
+    <t>onnx__Unsqueeze_1512</t>
+  </si>
+  <si>
+    <t>onnx__Unsqueeze_1537</t>
+  </si>
+  <si>
+    <t>onnx__Unsqueeze_1539</t>
+  </si>
+  <si>
+    <t>onnx__Unsqueeze_1541</t>
+  </si>
+  <si>
+    <t>onnx__Unsqueeze_1573</t>
+  </si>
+  <si>
+    <t>onnx__Unsqueeze_1575</t>
+  </si>
+  <si>
+    <t>onnx__Unsqueeze_1579</t>
+  </si>
+  <si>
+    <t>onnx__Unsqueeze_1597</t>
+  </si>
+  <si>
+    <t>onnx__Unsqueeze_1599</t>
+  </si>
+  <si>
+    <t>onnx__Unsqueeze_1603</t>
+  </si>
+  <si>
+    <t>onnx__Unsqueeze_1620</t>
+  </si>
+  <si>
+    <t>onnx__Unsqueeze_1622</t>
+  </si>
+  <si>
+    <t>onnx__Unsqueeze_1626</t>
+  </si>
+  <si>
+    <t>onnx__Unsqueeze_1651</t>
+  </si>
+  <si>
+    <t>onnx__Unsqueeze_1653</t>
+  </si>
+  <si>
+    <t>onnx__Unsqueeze_1655</t>
+  </si>
+  <si>
+    <t>onnx__Unsqueeze_1676</t>
+  </si>
+  <si>
+    <t>onnx__Unsqueeze_1678</t>
+  </si>
+  <si>
+    <t>onnx__Unsqueeze_1680</t>
+  </si>
+  <si>
+    <t>onnx__Unsqueeze_1682</t>
+  </si>
+  <si>
+    <t>onnx__Unsqueeze_871</t>
+  </si>
+  <si>
+    <t>onnx__Unsqueeze_873</t>
+  </si>
+  <si>
+    <t>onnx__Unsqueeze_877</t>
+  </si>
+  <si>
+    <t>onnx__Unsqueeze_895</t>
+  </si>
+  <si>
+    <t>onnx__Unsqueeze_897</t>
+  </si>
+  <si>
+    <t>onnx__Unsqueeze_901</t>
+  </si>
+  <si>
+    <t>onnx__Unsqueeze_918</t>
+  </si>
+  <si>
+    <t>onnx__Unsqueeze_920</t>
+  </si>
+  <si>
+    <t>onnx__Unsqueeze_924</t>
+  </si>
+  <si>
+    <t>onnx__Unsqueeze_949</t>
+  </si>
+  <si>
+    <t>onnx__Unsqueeze_951</t>
+  </si>
+  <si>
+    <t>onnx__Unsqueeze_953</t>
+  </si>
+  <si>
+    <t>onnx__Unsqueeze_985</t>
+  </si>
+  <si>
+    <t>onnx__Unsqueeze_987</t>
+  </si>
+  <si>
+    <t>onnx__Unsqueeze_991</t>
+  </si>
+  <si>
+    <t>x_Constant_17_output</t>
+  </si>
+  <si>
+    <t>x_Constant_19_output</t>
+  </si>
+  <si>
+    <t>x_Constant_26_output</t>
+  </si>
+  <si>
+    <t>x_Constant_27_output</t>
+  </si>
+  <si>
+    <t>x_Constant_28_output</t>
+  </si>
+  <si>
+    <t>x_Constant_42_output</t>
+  </si>
+  <si>
+    <t>x_Constant_43_output</t>
+  </si>
+  <si>
+    <t>x_Constant_44_output</t>
+  </si>
+  <si>
+    <t>x_Constant_65_output</t>
+  </si>
+  <si>
+    <t>x_Constant_66_output</t>
+  </si>
+  <si>
+    <t>x_Constant_67_output</t>
+  </si>
+  <si>
+    <t>x_Constant_68_output</t>
+  </si>
+  <si>
+    <t>x_Constant_6_output_</t>
+  </si>
+  <si>
+    <t>x_pe_layer_Constan_1</t>
+  </si>
+  <si>
+    <t>2x64x64 dlarray</t>
+  </si>
+  <si>
+    <t>Cast_To_CastLayer1054</t>
+  </si>
+  <si>
+    <t>onnx__Unsqueeze_1828</t>
+  </si>
+  <si>
+    <t>onnx__Unsqueeze_1830</t>
+  </si>
+  <si>
+    <t>Erf_To_ResizeLayer1135</t>
+  </si>
+  <si>
+    <t>onnx__Unsqueeze_1769</t>
+  </si>
+  <si>
+    <t>onnx__Unsqueeze_1771</t>
+  </si>
+  <si>
+    <t>onnx__Unsqueeze_1773</t>
+  </si>
+  <si>
+    <t>onnx__Unsqueeze_1778</t>
+  </si>
+  <si>
+    <t>onnx__Unsqueeze_1782</t>
+  </si>
+  <si>
+    <t>onnx__Unsqueeze_1784</t>
+  </si>
+  <si>
+    <t>'image_embeddings'</t>
+  </si>
+  <si>
+    <t>'point_coords'</t>
+  </si>
+  <si>
+    <t>'point_labels'</t>
+  </si>
+  <si>
+    <t>'has_mask_input'</t>
+  </si>
+  <si>
+    <t>'orig_im_size'</t>
   </si>
 </sst>
 </file>
@@ -676,13 +1288,11 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:B56"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D3" sqref="D3"/>
-    </sheetView>
+    <sheetView topLeftCell="A22" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="40.44140625" customWidth="1"/>
+    <col min="1" max="1" width="61.109375" customWidth="1"/>
     <col min="2" max="2" width="50.109375" customWidth="1"/>
   </cols>
   <sheetData>
@@ -1140,12 +1750,2353 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4395F91A-76D0-4770-9EC2-57016E662D6D}">
+  <dimension ref="A1:C205"/>
+  <sheetViews>
+    <sheetView tabSelected="1" topLeftCell="A70" workbookViewId="0">
+      <selection activeCell="A24" sqref="A24"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="48.6640625" customWidth="1"/>
+    <col min="2" max="2" width="22" customWidth="1"/>
+    <col min="3" max="3" width="27.5546875" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A1" s="1" t="s">
+        <v>105</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>105</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A2" s="1" t="s">
+        <v>105</v>
+      </c>
+      <c r="B2" s="1" t="s">
+        <v>105</v>
+      </c>
+      <c r="C2" s="1" t="s">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A3" s="1" t="s">
+        <v>105</v>
+      </c>
+      <c r="B3" s="1" t="s">
+        <v>105</v>
+      </c>
+      <c r="C3" s="1" t="s">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A4" s="1" t="s">
+        <v>105</v>
+      </c>
+      <c r="B4" s="1" t="s">
+        <v>105</v>
+      </c>
+      <c r="C4" s="1" t="s">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A5" s="1" t="s">
+        <v>105</v>
+      </c>
+      <c r="B5" s="1" t="s">
+        <v>105</v>
+      </c>
+      <c r="C5" s="1" t="s">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A6" s="1" t="s">
+        <v>105</v>
+      </c>
+      <c r="B6" s="1" t="s">
+        <v>105</v>
+      </c>
+      <c r="C6" s="1" t="s">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A7" s="1" t="s">
+        <v>105</v>
+      </c>
+      <c r="B7" s="1" t="s">
+        <v>105</v>
+      </c>
+      <c r="C7" s="1" t="s">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A8" s="1" t="s">
+        <v>105</v>
+      </c>
+      <c r="B8" s="1" t="s">
+        <v>105</v>
+      </c>
+      <c r="C8" s="1" t="s">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A9" s="1" t="s">
+        <v>105</v>
+      </c>
+      <c r="B9" s="1" t="s">
+        <v>105</v>
+      </c>
+      <c r="C9" s="1" t="s">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="10" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A10" s="1" t="s">
+        <v>105</v>
+      </c>
+      <c r="B10" s="1" t="s">
+        <v>105</v>
+      </c>
+      <c r="C10" s="1" t="s">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="11" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A11" s="1" t="s">
+        <v>105</v>
+      </c>
+      <c r="B11" s="1" t="s">
+        <v>105</v>
+      </c>
+      <c r="C11" s="1" t="s">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="12" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A12" s="1" t="s">
+        <v>105</v>
+      </c>
+      <c r="B12" s="1" t="s">
+        <v>105</v>
+      </c>
+      <c r="C12" s="1" t="s">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="13" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A13" s="1" t="s">
+        <v>105</v>
+      </c>
+      <c r="B13" s="1" t="s">
+        <v>105</v>
+      </c>
+      <c r="C13" s="1" t="s">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="14" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A14" s="1" t="s">
+        <v>105</v>
+      </c>
+      <c r="B14" s="1" t="s">
+        <v>105</v>
+      </c>
+      <c r="C14" s="1" t="s">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="15" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A15" s="1" t="s">
+        <v>105</v>
+      </c>
+      <c r="B15" s="1" t="s">
+        <v>105</v>
+      </c>
+      <c r="C15" s="1" t="s">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="16" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A16" s="1" t="s">
+        <v>105</v>
+      </c>
+      <c r="B16" s="1" t="s">
+        <v>105</v>
+      </c>
+      <c r="C16" s="1" t="s">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="17" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A17" s="1" t="s">
+        <v>105</v>
+      </c>
+      <c r="B17" s="1" t="s">
+        <v>105</v>
+      </c>
+      <c r="C17" s="1" t="s">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="18" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A18" s="1" t="s">
+        <v>105</v>
+      </c>
+      <c r="B18" s="1" t="s">
+        <v>105</v>
+      </c>
+      <c r="C18" s="1" t="s">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="19" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A19" s="1" t="s">
+        <v>105</v>
+      </c>
+      <c r="B19" s="1" t="s">
+        <v>105</v>
+      </c>
+      <c r="C19" s="1" t="s">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="20" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A20" s="1" t="s">
+        <v>105</v>
+      </c>
+      <c r="B20" s="1" t="s">
+        <v>105</v>
+      </c>
+      <c r="C20" s="1" t="s">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="21" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A21" s="1" t="s">
+        <v>105</v>
+      </c>
+      <c r="B21" s="1" t="s">
+        <v>105</v>
+      </c>
+      <c r="C21" s="1" t="s">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="22" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A22" s="1" t="s">
+        <v>105</v>
+      </c>
+      <c r="B22" s="1" t="s">
+        <v>105</v>
+      </c>
+      <c r="C22" s="1" t="s">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="23" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A23" s="1" t="s">
+        <v>105</v>
+      </c>
+      <c r="B23" s="1" t="s">
+        <v>105</v>
+      </c>
+      <c r="C23" s="1" t="s">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="24" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A24" s="1" t="s">
+        <v>106</v>
+      </c>
+      <c r="B24" s="1" t="s">
+        <v>107</v>
+      </c>
+      <c r="C24" s="1" t="s">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="25" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A25" s="1" t="s">
+        <v>106</v>
+      </c>
+      <c r="B25" s="1" t="s">
+        <v>109</v>
+      </c>
+      <c r="C25" s="1" t="s">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="26" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A26" s="1" t="s">
+        <v>106</v>
+      </c>
+      <c r="B26" s="1" t="s">
+        <v>111</v>
+      </c>
+      <c r="C26" s="1" t="s">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="27" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A27" s="1" t="s">
+        <v>106</v>
+      </c>
+      <c r="B27" s="1" t="s">
+        <v>112</v>
+      </c>
+      <c r="C27" s="1" t="s">
+        <v>113</v>
+      </c>
+    </row>
+    <row r="28" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A28" s="1" t="s">
+        <v>106</v>
+      </c>
+      <c r="B28" s="1" t="s">
+        <v>114</v>
+      </c>
+      <c r="C28" s="1" t="s">
+        <v>115</v>
+      </c>
+    </row>
+    <row r="29" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A29" s="1" t="s">
+        <v>106</v>
+      </c>
+      <c r="B29" s="1" t="s">
+        <v>116</v>
+      </c>
+      <c r="C29" s="1" t="s">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="30" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A30" s="1" t="s">
+        <v>106</v>
+      </c>
+      <c r="B30" s="1" t="s">
+        <v>117</v>
+      </c>
+      <c r="C30" s="1" t="s">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="31" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A31" s="1" t="s">
+        <v>106</v>
+      </c>
+      <c r="B31" s="1" t="s">
+        <v>118</v>
+      </c>
+      <c r="C31" s="1" t="s">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="32" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A32" s="1" t="s">
+        <v>106</v>
+      </c>
+      <c r="B32" s="1" t="s">
+        <v>119</v>
+      </c>
+      <c r="C32" s="1" t="s">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="33" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A33" s="1" t="s">
+        <v>106</v>
+      </c>
+      <c r="B33" s="1" t="s">
+        <v>120</v>
+      </c>
+      <c r="C33" s="1" t="s">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="34" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A34" s="1" t="s">
+        <v>106</v>
+      </c>
+      <c r="B34" s="1" t="s">
+        <v>121</v>
+      </c>
+      <c r="C34" s="1" t="s">
+        <v>113</v>
+      </c>
+    </row>
+    <row r="35" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A35" s="1" t="s">
+        <v>106</v>
+      </c>
+      <c r="B35" s="1" t="s">
+        <v>122</v>
+      </c>
+      <c r="C35" s="1" t="s">
+        <v>115</v>
+      </c>
+    </row>
+    <row r="36" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A36" s="1" t="s">
+        <v>106</v>
+      </c>
+      <c r="B36" s="1" t="s">
+        <v>123</v>
+      </c>
+      <c r="C36" s="1" t="s">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="37" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A37" s="1" t="s">
+        <v>106</v>
+      </c>
+      <c r="B37" s="1" t="s">
+        <v>124</v>
+      </c>
+      <c r="C37" s="1" t="s">
+        <v>113</v>
+      </c>
+    </row>
+    <row r="38" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A38" s="1" t="s">
+        <v>106</v>
+      </c>
+      <c r="B38" s="1" t="s">
+        <v>125</v>
+      </c>
+      <c r="C38" s="1" t="s">
+        <v>115</v>
+      </c>
+    </row>
+    <row r="39" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A39" s="1" t="s">
+        <v>106</v>
+      </c>
+      <c r="B39" s="1" t="s">
+        <v>126</v>
+      </c>
+      <c r="C39" s="1" t="s">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="40" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A40" s="1" t="s">
+        <v>106</v>
+      </c>
+      <c r="B40" s="1" t="s">
+        <v>127</v>
+      </c>
+      <c r="C40" s="1" t="s">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="41" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A41" s="1" t="s">
+        <v>106</v>
+      </c>
+      <c r="B41" s="1" t="s">
+        <v>128</v>
+      </c>
+      <c r="C41" s="1" t="s">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="42" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A42" s="1" t="s">
+        <v>106</v>
+      </c>
+      <c r="B42" s="1" t="s">
+        <v>129</v>
+      </c>
+      <c r="C42" s="1" t="s">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="43" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A43" s="1" t="s">
+        <v>106</v>
+      </c>
+      <c r="B43" s="1" t="s">
+        <v>130</v>
+      </c>
+      <c r="C43" s="1" t="s">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="44" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A44" s="1" t="s">
+        <v>106</v>
+      </c>
+      <c r="B44" s="1" t="s">
+        <v>131</v>
+      </c>
+      <c r="C44" s="1" t="s">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="45" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A45" s="1" t="s">
+        <v>106</v>
+      </c>
+      <c r="B45" s="1" t="s">
+        <v>132</v>
+      </c>
+      <c r="C45" s="1" t="s">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="46" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A46" s="1" t="s">
+        <v>106</v>
+      </c>
+      <c r="B46" s="1" t="s">
+        <v>133</v>
+      </c>
+      <c r="C46" s="1" t="s">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="47" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A47" s="1" t="s">
+        <v>106</v>
+      </c>
+      <c r="B47" s="1" t="s">
+        <v>134</v>
+      </c>
+      <c r="C47" s="1" t="s">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="48" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A48" s="1" t="s">
+        <v>106</v>
+      </c>
+      <c r="B48" s="1" t="s">
+        <v>135</v>
+      </c>
+      <c r="C48" s="1" t="s">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="49" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A49" s="1" t="s">
+        <v>106</v>
+      </c>
+      <c r="B49" s="1" t="s">
+        <v>136</v>
+      </c>
+      <c r="C49" s="1" t="s">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="50" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A50" s="1" t="s">
+        <v>106</v>
+      </c>
+      <c r="B50" s="1" t="s">
+        <v>137</v>
+      </c>
+      <c r="C50" s="1" t="s">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="51" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A51" s="1" t="s">
+        <v>106</v>
+      </c>
+      <c r="B51" s="1" t="s">
+        <v>138</v>
+      </c>
+      <c r="C51" s="1" t="s">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="52" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A52" s="1" t="s">
+        <v>106</v>
+      </c>
+      <c r="B52" s="1" t="s">
+        <v>139</v>
+      </c>
+      <c r="C52" s="1" t="s">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="53" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A53" s="1" t="s">
+        <v>106</v>
+      </c>
+      <c r="B53" s="1" t="s">
+        <v>140</v>
+      </c>
+      <c r="C53" s="1" t="s">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="54" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A54" s="1" t="s">
+        <v>106</v>
+      </c>
+      <c r="B54" s="1" t="s">
+        <v>141</v>
+      </c>
+      <c r="C54" s="1" t="s">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="55" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A55" s="1" t="s">
+        <v>106</v>
+      </c>
+      <c r="B55" s="1" t="s">
+        <v>142</v>
+      </c>
+      <c r="C55" s="1" t="s">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="56" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A56" s="1" t="s">
+        <v>106</v>
+      </c>
+      <c r="B56" s="1" t="s">
+        <v>143</v>
+      </c>
+      <c r="C56" s="1" t="s">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="57" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A57" s="1" t="s">
+        <v>106</v>
+      </c>
+      <c r="B57" s="1" t="s">
+        <v>144</v>
+      </c>
+      <c r="C57" s="1" t="s">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="58" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A58" s="1" t="s">
+        <v>106</v>
+      </c>
+      <c r="B58" s="1" t="s">
+        <v>145</v>
+      </c>
+      <c r="C58" s="1" t="s">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="59" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A59" s="1" t="s">
+        <v>106</v>
+      </c>
+      <c r="B59" s="1" t="s">
+        <v>146</v>
+      </c>
+      <c r="C59" s="1" t="s">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="60" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A60" s="1" t="s">
+        <v>106</v>
+      </c>
+      <c r="B60" s="1" t="s">
+        <v>147</v>
+      </c>
+      <c r="C60" s="1" t="s">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="61" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A61" s="1" t="s">
+        <v>106</v>
+      </c>
+      <c r="B61" s="1" t="s">
+        <v>148</v>
+      </c>
+      <c r="C61" s="1" t="s">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="62" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A62" s="1" t="s">
+        <v>106</v>
+      </c>
+      <c r="B62" s="1" t="s">
+        <v>149</v>
+      </c>
+      <c r="C62" s="1" t="s">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="63" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A63" s="1" t="s">
+        <v>106</v>
+      </c>
+      <c r="B63" s="1" t="s">
+        <v>151</v>
+      </c>
+      <c r="C63" s="1" t="s">
+        <v>152</v>
+      </c>
+    </row>
+    <row r="64" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A64" s="1" t="s">
+        <v>106</v>
+      </c>
+      <c r="B64" s="1" t="s">
+        <v>153</v>
+      </c>
+      <c r="C64" s="1" t="s">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="65" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A65" s="1" t="s">
+        <v>106</v>
+      </c>
+      <c r="B65" s="1" t="s">
+        <v>154</v>
+      </c>
+      <c r="C65" s="1" t="s">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="66" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A66" s="1" t="s">
+        <v>106</v>
+      </c>
+      <c r="B66" s="1" t="s">
+        <v>155</v>
+      </c>
+      <c r="C66" s="1" t="s">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="67" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A67" s="1" t="s">
+        <v>106</v>
+      </c>
+      <c r="B67" s="1" t="s">
+        <v>156</v>
+      </c>
+      <c r="C67" s="1" t="s">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="68" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A68" s="1" t="s">
+        <v>106</v>
+      </c>
+      <c r="B68" s="1" t="s">
+        <v>157</v>
+      </c>
+      <c r="C68" s="1" t="s">
+        <v>158</v>
+      </c>
+    </row>
+    <row r="69" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A69" s="1" t="s">
+        <v>106</v>
+      </c>
+      <c r="B69" s="1" t="s">
+        <v>159</v>
+      </c>
+      <c r="C69" s="1" t="s">
+        <v>158</v>
+      </c>
+    </row>
+    <row r="70" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A70" s="1" t="s">
+        <v>106</v>
+      </c>
+      <c r="B70" s="1" t="s">
+        <v>160</v>
+      </c>
+      <c r="C70" s="1" t="s">
+        <v>158</v>
+      </c>
+    </row>
+    <row r="71" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A71" s="1" t="s">
+        <v>106</v>
+      </c>
+      <c r="B71" s="1" t="s">
+        <v>161</v>
+      </c>
+      <c r="C71" s="1" t="s">
+        <v>162</v>
+      </c>
+    </row>
+    <row r="72" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A72" s="1" t="s">
+        <v>106</v>
+      </c>
+      <c r="B72" s="1" t="s">
+        <v>163</v>
+      </c>
+      <c r="C72" s="1" t="s">
+        <v>164</v>
+      </c>
+    </row>
+    <row r="73" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A73" s="1" t="s">
+        <v>106</v>
+      </c>
+      <c r="B73" s="1" t="s">
+        <v>165</v>
+      </c>
+      <c r="C73" s="1" t="s">
+        <v>166</v>
+      </c>
+    </row>
+    <row r="74" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A74" s="1" t="s">
+        <v>106</v>
+      </c>
+      <c r="B74" s="1" t="s">
+        <v>167</v>
+      </c>
+      <c r="C74" s="1" t="s">
+        <v>158</v>
+      </c>
+    </row>
+    <row r="75" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A75" s="1" t="s">
+        <v>106</v>
+      </c>
+      <c r="B75" s="1" t="s">
+        <v>168</v>
+      </c>
+      <c r="C75" s="1" t="s">
+        <v>158</v>
+      </c>
+    </row>
+    <row r="76" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A76" s="1" t="s">
+        <v>106</v>
+      </c>
+      <c r="B76" s="1" t="s">
+        <v>169</v>
+      </c>
+      <c r="C76" s="1" t="s">
+        <v>158</v>
+      </c>
+    </row>
+    <row r="77" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A77" s="1" t="s">
+        <v>106</v>
+      </c>
+      <c r="B77" s="1" t="s">
+        <v>170</v>
+      </c>
+      <c r="C77" s="1" t="s">
+        <v>162</v>
+      </c>
+    </row>
+    <row r="78" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A78" s="1" t="s">
+        <v>106</v>
+      </c>
+      <c r="B78" s="1" t="s">
+        <v>171</v>
+      </c>
+      <c r="C78" s="1" t="s">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="79" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A79" s="1" t="s">
+        <v>106</v>
+      </c>
+      <c r="B79" s="1" t="s">
+        <v>172</v>
+      </c>
+      <c r="C79" s="1" t="s">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="80" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A80" s="1" t="s">
+        <v>106</v>
+      </c>
+      <c r="B80" s="1" t="s">
+        <v>173</v>
+      </c>
+      <c r="C80" s="1" t="s">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="81" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A81" s="1" t="s">
+        <v>106</v>
+      </c>
+      <c r="B81" s="1" t="s">
+        <v>174</v>
+      </c>
+      <c r="C81" s="1" t="s">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="82" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A82" s="1" t="s">
+        <v>106</v>
+      </c>
+      <c r="B82" s="1" t="s">
+        <v>175</v>
+      </c>
+      <c r="C82" s="1" t="s">
+        <v>158</v>
+      </c>
+    </row>
+    <row r="83" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A83" s="1" t="s">
+        <v>106</v>
+      </c>
+      <c r="B83" s="1" t="s">
+        <v>176</v>
+      </c>
+      <c r="C83" s="1" t="s">
+        <v>158</v>
+      </c>
+    </row>
+    <row r="84" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A84" s="1" t="s">
+        <v>106</v>
+      </c>
+      <c r="B84" s="1" t="s">
+        <v>177</v>
+      </c>
+      <c r="C84" s="1" t="s">
+        <v>158</v>
+      </c>
+    </row>
+    <row r="85" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A85" s="1" t="s">
+        <v>106</v>
+      </c>
+      <c r="B85" s="1" t="s">
+        <v>178</v>
+      </c>
+      <c r="C85" s="1" t="s">
+        <v>162</v>
+      </c>
+    </row>
+    <row r="86" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A86" s="1" t="s">
+        <v>106</v>
+      </c>
+      <c r="B86" s="1" t="s">
+        <v>179</v>
+      </c>
+      <c r="C86" s="1" t="s">
+        <v>164</v>
+      </c>
+    </row>
+    <row r="87" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A87" s="1" t="s">
+        <v>106</v>
+      </c>
+      <c r="B87" s="1" t="s">
+        <v>180</v>
+      </c>
+      <c r="C87" s="1" t="s">
+        <v>166</v>
+      </c>
+    </row>
+    <row r="88" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A88" s="1" t="s">
+        <v>106</v>
+      </c>
+      <c r="B88" s="1" t="s">
+        <v>181</v>
+      </c>
+      <c r="C88" s="1" t="s">
+        <v>158</v>
+      </c>
+    </row>
+    <row r="89" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A89" s="1" t="s">
+        <v>106</v>
+      </c>
+      <c r="B89" s="1" t="s">
+        <v>182</v>
+      </c>
+      <c r="C89" s="1" t="s">
+        <v>158</v>
+      </c>
+    </row>
+    <row r="90" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A90" s="1" t="s">
+        <v>106</v>
+      </c>
+      <c r="B90" s="1" t="s">
+        <v>183</v>
+      </c>
+      <c r="C90" s="1" t="s">
+        <v>158</v>
+      </c>
+    </row>
+    <row r="91" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A91" s="1" t="s">
+        <v>106</v>
+      </c>
+      <c r="B91" s="1" t="s">
+        <v>184</v>
+      </c>
+      <c r="C91" s="1" t="s">
+        <v>162</v>
+      </c>
+    </row>
+    <row r="92" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A92" s="1" t="s">
+        <v>106</v>
+      </c>
+      <c r="B92" s="1" t="s">
+        <v>185</v>
+      </c>
+      <c r="C92" s="1" t="s">
+        <v>158</v>
+      </c>
+    </row>
+    <row r="93" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A93" s="1" t="s">
+        <v>106</v>
+      </c>
+      <c r="B93" s="1" t="s">
+        <v>186</v>
+      </c>
+      <c r="C93" s="1" t="s">
+        <v>158</v>
+      </c>
+    </row>
+    <row r="94" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A94" s="1" t="s">
+        <v>106</v>
+      </c>
+      <c r="B94" s="1" t="s">
+        <v>187</v>
+      </c>
+      <c r="C94" s="1" t="s">
+        <v>158</v>
+      </c>
+    </row>
+    <row r="95" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A95" s="1" t="s">
+        <v>106</v>
+      </c>
+      <c r="B95" s="1" t="s">
+        <v>188</v>
+      </c>
+      <c r="C95" s="1" t="s">
+        <v>162</v>
+      </c>
+    </row>
+    <row r="96" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A96" s="1" t="s">
+        <v>106</v>
+      </c>
+      <c r="B96" s="1" t="s">
+        <v>189</v>
+      </c>
+      <c r="C96" s="1" t="s">
+        <v>190</v>
+      </c>
+    </row>
+    <row r="97" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A97" s="1" t="s">
+        <v>106</v>
+      </c>
+      <c r="B97" s="1" t="s">
+        <v>191</v>
+      </c>
+      <c r="C97" s="1" t="s">
+        <v>190</v>
+      </c>
+    </row>
+    <row r="98" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A98" s="1" t="s">
+        <v>106</v>
+      </c>
+      <c r="B98" s="1" t="s">
+        <v>192</v>
+      </c>
+      <c r="C98" s="1" t="s">
+        <v>190</v>
+      </c>
+    </row>
+    <row r="99" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A99" s="1" t="s">
+        <v>106</v>
+      </c>
+      <c r="B99" s="1" t="s">
+        <v>193</v>
+      </c>
+      <c r="C99" s="1" t="s">
+        <v>190</v>
+      </c>
+    </row>
+    <row r="100" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A100" s="1" t="s">
+        <v>106</v>
+      </c>
+      <c r="B100" s="1" t="s">
+        <v>194</v>
+      </c>
+      <c r="C100" s="1" t="s">
+        <v>190</v>
+      </c>
+    </row>
+    <row r="101" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A101" s="1" t="s">
+        <v>106</v>
+      </c>
+      <c r="B101" s="1" t="s">
+        <v>195</v>
+      </c>
+      <c r="C101" s="1" t="s">
+        <v>190</v>
+      </c>
+    </row>
+    <row r="102" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A102" s="1" t="s">
+        <v>106</v>
+      </c>
+      <c r="B102" s="1" t="s">
+        <v>196</v>
+      </c>
+      <c r="C102" s="1" t="s">
+        <v>190</v>
+      </c>
+    </row>
+    <row r="103" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A103" s="1" t="s">
+        <v>106</v>
+      </c>
+      <c r="B103" s="1" t="s">
+        <v>197</v>
+      </c>
+      <c r="C103" s="1" t="s">
+        <v>190</v>
+      </c>
+    </row>
+    <row r="104" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A104" s="1" t="s">
+        <v>106</v>
+      </c>
+      <c r="B104" s="1" t="s">
+        <v>198</v>
+      </c>
+      <c r="C104" s="1" t="s">
+        <v>190</v>
+      </c>
+    </row>
+    <row r="105" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A105" s="1" t="s">
+        <v>106</v>
+      </c>
+      <c r="B105" s="1" t="s">
+        <v>199</v>
+      </c>
+      <c r="C105" s="1" t="s">
+        <v>190</v>
+      </c>
+    </row>
+    <row r="106" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A106" s="1" t="s">
+        <v>106</v>
+      </c>
+      <c r="B106" s="1" t="s">
+        <v>200</v>
+      </c>
+      <c r="C106" s="1" t="s">
+        <v>190</v>
+      </c>
+    </row>
+    <row r="107" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A107" s="1" t="s">
+        <v>106</v>
+      </c>
+      <c r="B107" s="1" t="s">
+        <v>201</v>
+      </c>
+      <c r="C107" s="1" t="s">
+        <v>190</v>
+      </c>
+    </row>
+    <row r="108" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A108" s="1" t="s">
+        <v>106</v>
+      </c>
+      <c r="B108" s="1" t="s">
+        <v>202</v>
+      </c>
+      <c r="C108" s="1" t="s">
+        <v>190</v>
+      </c>
+    </row>
+    <row r="109" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A109" s="1" t="s">
+        <v>106</v>
+      </c>
+      <c r="B109" s="1" t="s">
+        <v>203</v>
+      </c>
+      <c r="C109" s="1" t="s">
+        <v>190</v>
+      </c>
+    </row>
+    <row r="110" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A110" s="1" t="s">
+        <v>106</v>
+      </c>
+      <c r="B110" s="1" t="s">
+        <v>204</v>
+      </c>
+      <c r="C110" s="1" t="s">
+        <v>190</v>
+      </c>
+    </row>
+    <row r="111" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A111" s="1" t="s">
+        <v>106</v>
+      </c>
+      <c r="B111" s="1" t="s">
+        <v>205</v>
+      </c>
+      <c r="C111" s="1" t="s">
+        <v>190</v>
+      </c>
+    </row>
+    <row r="112" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A112" s="1" t="s">
+        <v>106</v>
+      </c>
+      <c r="B112" s="1" t="s">
+        <v>206</v>
+      </c>
+      <c r="C112" s="1" t="s">
+        <v>190</v>
+      </c>
+    </row>
+    <row r="113" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A113" s="1" t="s">
+        <v>106</v>
+      </c>
+      <c r="B113" s="1" t="s">
+        <v>207</v>
+      </c>
+      <c r="C113" s="1" t="s">
+        <v>190</v>
+      </c>
+    </row>
+    <row r="114" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A114" s="1" t="s">
+        <v>106</v>
+      </c>
+      <c r="B114" s="1" t="s">
+        <v>208</v>
+      </c>
+      <c r="C114" s="1" t="s">
+        <v>190</v>
+      </c>
+    </row>
+    <row r="115" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A115" s="1" t="s">
+        <v>106</v>
+      </c>
+      <c r="B115" s="1" t="s">
+        <v>209</v>
+      </c>
+      <c r="C115" s="1" t="s">
+        <v>190</v>
+      </c>
+    </row>
+    <row r="116" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A116" s="1" t="s">
+        <v>106</v>
+      </c>
+      <c r="B116" s="1" t="s">
+        <v>210</v>
+      </c>
+      <c r="C116" s="1" t="s">
+        <v>190</v>
+      </c>
+    </row>
+    <row r="117" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A117" s="1" t="s">
+        <v>106</v>
+      </c>
+      <c r="B117" s="1" t="s">
+        <v>211</v>
+      </c>
+      <c r="C117" s="1" t="s">
+        <v>190</v>
+      </c>
+    </row>
+    <row r="118" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A118" s="1" t="s">
+        <v>106</v>
+      </c>
+      <c r="B118" s="1" t="s">
+        <v>212</v>
+      </c>
+      <c r="C118" s="1" t="s">
+        <v>190</v>
+      </c>
+    </row>
+    <row r="119" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A119" s="1" t="s">
+        <v>106</v>
+      </c>
+      <c r="B119" s="1" t="s">
+        <v>213</v>
+      </c>
+      <c r="C119" s="1" t="s">
+        <v>190</v>
+      </c>
+    </row>
+    <row r="120" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A120" s="1" t="s">
+        <v>106</v>
+      </c>
+      <c r="B120" s="1" t="s">
+        <v>214</v>
+      </c>
+      <c r="C120" s="1" t="s">
+        <v>190</v>
+      </c>
+    </row>
+    <row r="121" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A121" s="1" t="s">
+        <v>106</v>
+      </c>
+      <c r="B121" s="1" t="s">
+        <v>215</v>
+      </c>
+      <c r="C121" s="1" t="s">
+        <v>190</v>
+      </c>
+    </row>
+    <row r="122" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A122" s="1" t="s">
+        <v>106</v>
+      </c>
+      <c r="B122" s="1" t="s">
+        <v>216</v>
+      </c>
+      <c r="C122" s="1" t="s">
+        <v>190</v>
+      </c>
+    </row>
+    <row r="123" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A123" s="1" t="s">
+        <v>106</v>
+      </c>
+      <c r="B123" s="1" t="s">
+        <v>217</v>
+      </c>
+      <c r="C123" s="1" t="s">
+        <v>190</v>
+      </c>
+    </row>
+    <row r="124" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A124" s="1" t="s">
+        <v>106</v>
+      </c>
+      <c r="B124" s="1" t="s">
+        <v>218</v>
+      </c>
+      <c r="C124" s="1" t="s">
+        <v>190</v>
+      </c>
+    </row>
+    <row r="125" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A125" s="1" t="s">
+        <v>106</v>
+      </c>
+      <c r="B125" s="1" t="s">
+        <v>219</v>
+      </c>
+      <c r="C125" s="1" t="s">
+        <v>190</v>
+      </c>
+    </row>
+    <row r="126" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A126" s="1" t="s">
+        <v>106</v>
+      </c>
+      <c r="B126" s="1" t="s">
+        <v>220</v>
+      </c>
+      <c r="C126" s="1" t="s">
+        <v>190</v>
+      </c>
+    </row>
+    <row r="127" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A127" s="1" t="s">
+        <v>106</v>
+      </c>
+      <c r="B127" s="1" t="s">
+        <v>221</v>
+      </c>
+      <c r="C127" s="1" t="s">
+        <v>190</v>
+      </c>
+    </row>
+    <row r="128" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A128" s="1" t="s">
+        <v>106</v>
+      </c>
+      <c r="B128" s="1" t="s">
+        <v>222</v>
+      </c>
+      <c r="C128" s="1" t="s">
+        <v>190</v>
+      </c>
+    </row>
+    <row r="129" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A129" s="1" t="s">
+        <v>106</v>
+      </c>
+      <c r="B129" s="1" t="s">
+        <v>223</v>
+      </c>
+      <c r="C129" s="1" t="s">
+        <v>190</v>
+      </c>
+    </row>
+    <row r="130" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A130" s="1" t="s">
+        <v>106</v>
+      </c>
+      <c r="B130" s="1" t="s">
+        <v>224</v>
+      </c>
+      <c r="C130" s="1" t="s">
+        <v>190</v>
+      </c>
+    </row>
+    <row r="131" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A131" s="1" t="s">
+        <v>106</v>
+      </c>
+      <c r="B131" s="1" t="s">
+        <v>225</v>
+      </c>
+      <c r="C131" s="1" t="s">
+        <v>190</v>
+      </c>
+    </row>
+    <row r="132" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A132" s="1" t="s">
+        <v>106</v>
+      </c>
+      <c r="B132" s="1" t="s">
+        <v>226</v>
+      </c>
+      <c r="C132" s="1" t="s">
+        <v>190</v>
+      </c>
+    </row>
+    <row r="133" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A133" s="1" t="s">
+        <v>106</v>
+      </c>
+      <c r="B133" s="1" t="s">
+        <v>227</v>
+      </c>
+      <c r="C133" s="1" t="s">
+        <v>190</v>
+      </c>
+    </row>
+    <row r="134" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A134" s="1" t="s">
+        <v>106</v>
+      </c>
+      <c r="B134" s="1" t="s">
+        <v>228</v>
+      </c>
+      <c r="C134" s="1" t="s">
+        <v>190</v>
+      </c>
+    </row>
+    <row r="135" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A135" s="1" t="s">
+        <v>106</v>
+      </c>
+      <c r="B135" s="1" t="s">
+        <v>229</v>
+      </c>
+      <c r="C135" s="1" t="s">
+        <v>190</v>
+      </c>
+    </row>
+    <row r="136" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A136" s="1" t="s">
+        <v>106</v>
+      </c>
+      <c r="B136" s="1" t="s">
+        <v>230</v>
+      </c>
+      <c r="C136" s="1" t="s">
+        <v>190</v>
+      </c>
+    </row>
+    <row r="137" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A137" s="1" t="s">
+        <v>106</v>
+      </c>
+      <c r="B137" s="1" t="s">
+        <v>231</v>
+      </c>
+      <c r="C137" s="1" t="s">
+        <v>190</v>
+      </c>
+    </row>
+    <row r="138" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A138" s="1" t="s">
+        <v>106</v>
+      </c>
+      <c r="B138" s="1" t="s">
+        <v>232</v>
+      </c>
+      <c r="C138" s="1" t="s">
+        <v>190</v>
+      </c>
+    </row>
+    <row r="139" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A139" s="1" t="s">
+        <v>106</v>
+      </c>
+      <c r="B139" s="1" t="s">
+        <v>233</v>
+      </c>
+      <c r="C139" s="1" t="s">
+        <v>190</v>
+      </c>
+    </row>
+    <row r="140" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A140" s="1" t="s">
+        <v>106</v>
+      </c>
+      <c r="B140" s="1" t="s">
+        <v>234</v>
+      </c>
+      <c r="C140" s="1" t="s">
+        <v>190</v>
+      </c>
+    </row>
+    <row r="141" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A141" s="1" t="s">
+        <v>106</v>
+      </c>
+      <c r="B141" s="1" t="s">
+        <v>235</v>
+      </c>
+      <c r="C141" s="1" t="s">
+        <v>190</v>
+      </c>
+    </row>
+    <row r="142" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A142" s="1" t="s">
+        <v>106</v>
+      </c>
+      <c r="B142" s="1" t="s">
+        <v>236</v>
+      </c>
+      <c r="C142" s="1" t="s">
+        <v>190</v>
+      </c>
+    </row>
+    <row r="143" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A143" s="1" t="s">
+        <v>106</v>
+      </c>
+      <c r="B143" s="1" t="s">
+        <v>237</v>
+      </c>
+      <c r="C143" s="1" t="s">
+        <v>190</v>
+      </c>
+    </row>
+    <row r="144" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A144" s="1" t="s">
+        <v>106</v>
+      </c>
+      <c r="B144" s="1" t="s">
+        <v>238</v>
+      </c>
+      <c r="C144" s="1" t="s">
+        <v>190</v>
+      </c>
+    </row>
+    <row r="145" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A145" s="1" t="s">
+        <v>106</v>
+      </c>
+      <c r="B145" s="1" t="s">
+        <v>239</v>
+      </c>
+      <c r="C145" s="1" t="s">
+        <v>190</v>
+      </c>
+    </row>
+    <row r="146" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A146" s="1" t="s">
+        <v>106</v>
+      </c>
+      <c r="B146" s="1" t="s">
+        <v>240</v>
+      </c>
+      <c r="C146" s="1" t="s">
+        <v>190</v>
+      </c>
+    </row>
+    <row r="147" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A147" s="1" t="s">
+        <v>106</v>
+      </c>
+      <c r="B147" s="1" t="s">
+        <v>241</v>
+      </c>
+      <c r="C147" s="1" t="s">
+        <v>190</v>
+      </c>
+    </row>
+    <row r="148" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A148" s="1" t="s">
+        <v>106</v>
+      </c>
+      <c r="B148" s="1" t="s">
+        <v>242</v>
+      </c>
+      <c r="C148" s="1" t="s">
+        <v>190</v>
+      </c>
+    </row>
+    <row r="149" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A149" s="1" t="s">
+        <v>106</v>
+      </c>
+      <c r="B149" s="1" t="s">
+        <v>243</v>
+      </c>
+      <c r="C149" s="1" t="s">
+        <v>190</v>
+      </c>
+    </row>
+    <row r="150" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A150" s="1" t="s">
+        <v>106</v>
+      </c>
+      <c r="B150" s="1" t="s">
+        <v>244</v>
+      </c>
+      <c r="C150" s="1" t="s">
+        <v>190</v>
+      </c>
+    </row>
+    <row r="151" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A151" s="1" t="s">
+        <v>106</v>
+      </c>
+      <c r="B151" s="1" t="s">
+        <v>245</v>
+      </c>
+      <c r="C151" s="1" t="s">
+        <v>190</v>
+      </c>
+    </row>
+    <row r="152" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A152" s="1" t="s">
+        <v>106</v>
+      </c>
+      <c r="B152" s="1" t="s">
+        <v>246</v>
+      </c>
+      <c r="C152" s="1" t="s">
+        <v>190</v>
+      </c>
+    </row>
+    <row r="153" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A153" s="1" t="s">
+        <v>106</v>
+      </c>
+      <c r="B153" s="1" t="s">
+        <v>247</v>
+      </c>
+      <c r="C153" s="1" t="s">
+        <v>190</v>
+      </c>
+    </row>
+    <row r="154" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A154" s="1" t="s">
+        <v>106</v>
+      </c>
+      <c r="B154" s="1" t="s">
+        <v>248</v>
+      </c>
+      <c r="C154" s="1" t="s">
+        <v>190</v>
+      </c>
+    </row>
+    <row r="155" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A155" s="1" t="s">
+        <v>106</v>
+      </c>
+      <c r="B155" s="1" t="s">
+        <v>249</v>
+      </c>
+      <c r="C155" s="1" t="s">
+        <v>190</v>
+      </c>
+    </row>
+    <row r="156" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A156" s="1" t="s">
+        <v>106</v>
+      </c>
+      <c r="B156" s="1" t="s">
+        <v>250</v>
+      </c>
+      <c r="C156" s="1" t="s">
+        <v>190</v>
+      </c>
+    </row>
+    <row r="157" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A157" s="1" t="s">
+        <v>106</v>
+      </c>
+      <c r="B157" s="1" t="s">
+        <v>251</v>
+      </c>
+      <c r="C157" s="1" t="s">
+        <v>190</v>
+      </c>
+    </row>
+    <row r="158" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A158" s="1" t="s">
+        <v>106</v>
+      </c>
+      <c r="B158" s="1" t="s">
+        <v>252</v>
+      </c>
+      <c r="C158" s="1" t="s">
+        <v>190</v>
+      </c>
+    </row>
+    <row r="159" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A159" s="1" t="s">
+        <v>106</v>
+      </c>
+      <c r="B159" s="1" t="s">
+        <v>253</v>
+      </c>
+      <c r="C159" s="1" t="s">
+        <v>190</v>
+      </c>
+    </row>
+    <row r="160" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A160" s="1" t="s">
+        <v>106</v>
+      </c>
+      <c r="B160" s="1" t="s">
+        <v>254</v>
+      </c>
+      <c r="C160" s="1" t="s">
+        <v>190</v>
+      </c>
+    </row>
+    <row r="161" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A161" s="1" t="s">
+        <v>106</v>
+      </c>
+      <c r="B161" s="1" t="s">
+        <v>255</v>
+      </c>
+      <c r="C161" s="1" t="s">
+        <v>190</v>
+      </c>
+    </row>
+    <row r="162" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A162" s="1" t="s">
+        <v>106</v>
+      </c>
+      <c r="B162" s="1" t="s">
+        <v>256</v>
+      </c>
+      <c r="C162" s="1" t="s">
+        <v>190</v>
+      </c>
+    </row>
+    <row r="163" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A163" s="1" t="s">
+        <v>106</v>
+      </c>
+      <c r="B163" s="1" t="s">
+        <v>257</v>
+      </c>
+      <c r="C163" s="1" t="s">
+        <v>190</v>
+      </c>
+    </row>
+    <row r="164" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A164" s="1" t="s">
+        <v>106</v>
+      </c>
+      <c r="B164" s="1" t="s">
+        <v>258</v>
+      </c>
+      <c r="C164" s="1" t="s">
+        <v>190</v>
+      </c>
+    </row>
+    <row r="165" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A165" s="1" t="s">
+        <v>106</v>
+      </c>
+      <c r="B165" s="1" t="s">
+        <v>259</v>
+      </c>
+      <c r="C165" s="1" t="s">
+        <v>190</v>
+      </c>
+    </row>
+    <row r="166" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A166" s="1" t="s">
+        <v>106</v>
+      </c>
+      <c r="B166" s="1" t="s">
+        <v>260</v>
+      </c>
+      <c r="C166" s="1" t="s">
+        <v>190</v>
+      </c>
+    </row>
+    <row r="167" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A167" s="1" t="s">
+        <v>106</v>
+      </c>
+      <c r="B167" s="1" t="s">
+        <v>261</v>
+      </c>
+      <c r="C167" s="1" t="s">
+        <v>190</v>
+      </c>
+    </row>
+    <row r="168" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A168" s="1" t="s">
+        <v>106</v>
+      </c>
+      <c r="B168" s="1" t="s">
+        <v>262</v>
+      </c>
+      <c r="C168" s="1" t="s">
+        <v>190</v>
+      </c>
+    </row>
+    <row r="169" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A169" s="1" t="s">
+        <v>106</v>
+      </c>
+      <c r="B169" s="1" t="s">
+        <v>263</v>
+      </c>
+      <c r="C169" s="1" t="s">
+        <v>190</v>
+      </c>
+    </row>
+    <row r="170" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A170" s="1" t="s">
+        <v>106</v>
+      </c>
+      <c r="B170" s="1" t="s">
+        <v>264</v>
+      </c>
+      <c r="C170" s="1" t="s">
+        <v>190</v>
+      </c>
+    </row>
+    <row r="171" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A171" s="1" t="s">
+        <v>106</v>
+      </c>
+      <c r="B171" s="1" t="s">
+        <v>265</v>
+      </c>
+      <c r="C171" s="1" t="s">
+        <v>190</v>
+      </c>
+    </row>
+    <row r="172" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A172" s="1" t="s">
+        <v>106</v>
+      </c>
+      <c r="B172" s="1" t="s">
+        <v>266</v>
+      </c>
+      <c r="C172" s="1" t="s">
+        <v>190</v>
+      </c>
+    </row>
+    <row r="173" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A173" s="1" t="s">
+        <v>106</v>
+      </c>
+      <c r="B173" s="1" t="s">
+        <v>267</v>
+      </c>
+      <c r="C173" s="1" t="s">
+        <v>190</v>
+      </c>
+    </row>
+    <row r="174" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A174" s="1" t="s">
+        <v>106</v>
+      </c>
+      <c r="B174" s="1" t="s">
+        <v>268</v>
+      </c>
+      <c r="C174" s="1" t="s">
+        <v>190</v>
+      </c>
+    </row>
+    <row r="175" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A175" s="1" t="s">
+        <v>106</v>
+      </c>
+      <c r="B175" s="1" t="s">
+        <v>269</v>
+      </c>
+      <c r="C175" s="1" t="s">
+        <v>190</v>
+      </c>
+    </row>
+    <row r="176" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A176" s="1" t="s">
+        <v>106</v>
+      </c>
+      <c r="B176" s="1" t="s">
+        <v>270</v>
+      </c>
+      <c r="C176" s="1" t="s">
+        <v>190</v>
+      </c>
+    </row>
+    <row r="177" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A177" s="1" t="s">
+        <v>106</v>
+      </c>
+      <c r="B177" s="1" t="s">
+        <v>271</v>
+      </c>
+      <c r="C177" s="1" t="s">
+        <v>190</v>
+      </c>
+    </row>
+    <row r="178" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A178" s="1" t="s">
+        <v>106</v>
+      </c>
+      <c r="B178" s="1" t="s">
+        <v>272</v>
+      </c>
+      <c r="C178" s="1" t="s">
+        <v>190</v>
+      </c>
+    </row>
+    <row r="179" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A179" s="1" t="s">
+        <v>106</v>
+      </c>
+      <c r="B179" s="1" t="s">
+        <v>273</v>
+      </c>
+      <c r="C179" s="1" t="s">
+        <v>190</v>
+      </c>
+    </row>
+    <row r="180" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A180" s="1" t="s">
+        <v>106</v>
+      </c>
+      <c r="B180" s="1" t="s">
+        <v>274</v>
+      </c>
+      <c r="C180" s="1" t="s">
+        <v>190</v>
+      </c>
+    </row>
+    <row r="181" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A181" s="1" t="s">
+        <v>106</v>
+      </c>
+      <c r="B181" s="1" t="s">
+        <v>275</v>
+      </c>
+      <c r="C181" s="1" t="s">
+        <v>190</v>
+      </c>
+    </row>
+    <row r="182" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A182" s="1" t="s">
+        <v>106</v>
+      </c>
+      <c r="B182" s="1" t="s">
+        <v>276</v>
+      </c>
+      <c r="C182" s="1" t="s">
+        <v>190</v>
+      </c>
+    </row>
+    <row r="183" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A183" s="1" t="s">
+        <v>106</v>
+      </c>
+      <c r="B183" s="1" t="s">
+        <v>277</v>
+      </c>
+      <c r="C183" s="1" t="s">
+        <v>190</v>
+      </c>
+    </row>
+    <row r="184" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A184" s="1" t="s">
+        <v>106</v>
+      </c>
+      <c r="B184" s="1" t="s">
+        <v>278</v>
+      </c>
+      <c r="C184" s="1" t="s">
+        <v>190</v>
+      </c>
+    </row>
+    <row r="185" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A185" s="1" t="s">
+        <v>106</v>
+      </c>
+      <c r="B185" s="1" t="s">
+        <v>279</v>
+      </c>
+      <c r="C185" s="1" t="s">
+        <v>190</v>
+      </c>
+    </row>
+    <row r="186" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A186" s="1" t="s">
+        <v>106</v>
+      </c>
+      <c r="B186" s="1" t="s">
+        <v>280</v>
+      </c>
+      <c r="C186" s="1" t="s">
+        <v>190</v>
+      </c>
+    </row>
+    <row r="187" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A187" s="1" t="s">
+        <v>106</v>
+      </c>
+      <c r="B187" s="1" t="s">
+        <v>281</v>
+      </c>
+      <c r="C187" s="1" t="s">
+        <v>190</v>
+      </c>
+    </row>
+    <row r="188" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A188" s="1" t="s">
+        <v>106</v>
+      </c>
+      <c r="B188" s="1" t="s">
+        <v>282</v>
+      </c>
+      <c r="C188" s="1" t="s">
+        <v>190</v>
+      </c>
+    </row>
+    <row r="189" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A189" s="1" t="s">
+        <v>106</v>
+      </c>
+      <c r="B189" s="1" t="s">
+        <v>283</v>
+      </c>
+      <c r="C189" s="1" t="s">
+        <v>190</v>
+      </c>
+    </row>
+    <row r="190" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A190" s="1" t="s">
+        <v>106</v>
+      </c>
+      <c r="B190" s="1" t="s">
+        <v>284</v>
+      </c>
+      <c r="C190" s="1" t="s">
+        <v>190</v>
+      </c>
+    </row>
+    <row r="191" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A191" s="1" t="s">
+        <v>106</v>
+      </c>
+      <c r="B191" s="1" t="s">
+        <v>285</v>
+      </c>
+      <c r="C191" s="1" t="s">
+        <v>190</v>
+      </c>
+    </row>
+    <row r="192" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A192" s="1" t="s">
+        <v>106</v>
+      </c>
+      <c r="B192" s="1" t="s">
+        <v>286</v>
+      </c>
+      <c r="C192" s="1" t="s">
+        <v>190</v>
+      </c>
+    </row>
+    <row r="193" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A193" s="1" t="s">
+        <v>106</v>
+      </c>
+      <c r="B193" s="1" t="s">
+        <v>287</v>
+      </c>
+      <c r="C193" s="1" t="s">
+        <v>190</v>
+      </c>
+    </row>
+    <row r="194" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A194" s="1" t="s">
+        <v>106</v>
+      </c>
+      <c r="B194" s="1" t="s">
+        <v>288</v>
+      </c>
+      <c r="C194" s="1" t="s">
+        <v>190</v>
+      </c>
+    </row>
+    <row r="195" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A195" s="1" t="s">
+        <v>106</v>
+      </c>
+      <c r="B195" s="1" t="s">
+        <v>289</v>
+      </c>
+      <c r="C195" s="1" t="s">
+        <v>190</v>
+      </c>
+    </row>
+    <row r="196" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A196" s="1" t="s">
+        <v>106</v>
+      </c>
+      <c r="B196" s="1" t="s">
+        <v>290</v>
+      </c>
+      <c r="C196" s="1" t="s">
+        <v>190</v>
+      </c>
+    </row>
+    <row r="197" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A197" s="1" t="s">
+        <v>106</v>
+      </c>
+      <c r="B197" s="1" t="s">
+        <v>291</v>
+      </c>
+      <c r="C197" s="1" t="s">
+        <v>292</v>
+      </c>
+    </row>
+    <row r="198" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A198" s="1" t="s">
+        <v>293</v>
+      </c>
+      <c r="B198" s="1" t="s">
+        <v>294</v>
+      </c>
+      <c r="C198" s="1" t="s">
+        <v>190</v>
+      </c>
+    </row>
+    <row r="199" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A199" s="1" t="s">
+        <v>293</v>
+      </c>
+      <c r="B199" s="1" t="s">
+        <v>295</v>
+      </c>
+      <c r="C199" s="1" t="s">
+        <v>190</v>
+      </c>
+    </row>
+    <row r="200" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A200" s="1" t="s">
+        <v>296</v>
+      </c>
+      <c r="B200" s="1" t="s">
+        <v>297</v>
+      </c>
+      <c r="C200" s="1" t="s">
+        <v>190</v>
+      </c>
+    </row>
+    <row r="201" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A201" s="1" t="s">
+        <v>296</v>
+      </c>
+      <c r="B201" s="1" t="s">
+        <v>298</v>
+      </c>
+      <c r="C201" s="1" t="s">
+        <v>190</v>
+      </c>
+    </row>
+    <row r="202" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A202" s="1" t="s">
+        <v>296</v>
+      </c>
+      <c r="B202" s="1" t="s">
+        <v>299</v>
+      </c>
+      <c r="C202" s="1" t="s">
+        <v>190</v>
+      </c>
+    </row>
+    <row r="203" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A203" s="1" t="s">
+        <v>296</v>
+      </c>
+      <c r="B203" s="1" t="s">
+        <v>300</v>
+      </c>
+      <c r="C203" s="1" t="s">
+        <v>190</v>
+      </c>
+    </row>
+    <row r="204" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A204" s="1" t="s">
+        <v>296</v>
+      </c>
+      <c r="B204" s="1" t="s">
+        <v>301</v>
+      </c>
+      <c r="C204" s="1" t="s">
+        <v>190</v>
+      </c>
+    </row>
+    <row r="205" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A205" s="1" t="s">
+        <v>296</v>
+      </c>
+      <c r="B205" s="1" t="s">
+        <v>302</v>
+      </c>
+      <c r="C205" s="1" t="s">
+        <v>190</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{AA1B7BA0-35BD-4B7A-8424-18C6221F2128}">
+  <dimension ref="A1:F1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="E15" sqref="E15"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetData>
+    <row r="1" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A1" s="1" t="s">
+        <v>303</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>304</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>305</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>306</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>307</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EC299E68-567C-436E-B5E4-76D785D7E611}">
+  <dimension ref="A1:D1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B9" sqref="B9"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="24.77734375" customWidth="1"/>
+    <col min="2" max="2" width="23.6640625" customWidth="1"/>
+    <col min="3" max="3" width="30" customWidth="1"/>
+    <col min="4" max="4" width="26" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A1" s="1" t="s">
+        <v>84</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>73</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>86</v>
+      </c>
+      <c r="D1" s="1"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{622644CD-A7D0-4964-A5E3-96BE6FDC9BA0}">
   <dimension ref="A1:A42"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C22" sqref="C22"/>
-    </sheetView>
+    <sheetView topLeftCell="A25" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>

</xml_diff>